<commit_message>
se arregla el metodo de creacion de parejas
</commit_message>
<xml_diff>
--- a/src/Palabras_Claves_Version_10-08-2024.xlsx
+++ b/src/Palabras_Claves_Version_10-08-2024.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sague\OneDrive\Escritorio\webScrappingFunding\WebScraping_Finding\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bc5085ef5d50236/Escritorio/webScrappingFunding/WebScraping_Finding/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96812710-EF7C-4AD3-8B22-7635FB3029BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{96812710-EF7C-4AD3-8B22-7635FB3029BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38FAF78E-B7B5-433B-ABC5-B4210840612F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{E42FA243-F694-480D-BC3A-A77E7821E5C9}"/>
   </bookViews>
@@ -1528,13 +1528,17 @@
   <cx:chart>
     <cx:plotArea>
       <cx:plotAreaRegion>
-        <cx:series layoutId="funnel" hidden="1" uniqueId="{F29B01F1-58D0-4A76-8CF1-27E2A53200D8}" formatIdx="0">
+        <cx:series layoutId="funnel" uniqueId="{F29B01F1-58D0-4A76-8CF1-27E2A53200D8}" formatIdx="0">
           <cx:dataLabels>
             <cx:visibility seriesName="0" categoryName="0" value="1"/>
           </cx:dataLabels>
           <cx:dataId val="0"/>
         </cx:series>
       </cx:plotAreaRegion>
+      <cx:axis id="1">
+        <cx:catScaling/>
+        <cx:tickLabels/>
+      </cx:axis>
     </cx:plotArea>
   </cx:chart>
   <cx:spPr>
@@ -2142,8 +2146,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8258175" y="2574607"/>
-              <a:ext cx="9408794" cy="2060258"/>
+              <a:off x="9725025" y="190500"/>
+              <a:ext cx="9408794" cy="190500"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2178,16 +2182,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6B9B1C01-571A-410E-9497-4A31E8E8EC12}" name="Tabla1" displayName="Tabla1" ref="A1:G373" totalsRowShown="0">
-  <autoFilter ref="A1:G373" xr:uid="{6B9B1C01-571A-410E-9497-4A31E8E8EC12}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="1"/>
-        <filter val="12"/>
-        <filter val="3"/>
-        <filter val="6"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G373" xr:uid="{6B9B1C01-571A-410E-9497-4A31E8E8EC12}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{B78181C8-1652-4E98-BB89-2778FF143DE9}" name="Investigador"/>
     <tableColumn id="2" xr3:uid="{9A39A5A2-88B6-480F-BB85-AE17A8B9B5F0}" name="Words" dataDxfId="1"/>
@@ -2522,7 +2517,7 @@
   <dimension ref="A1:Q373"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" workbookViewId="0">
-      <selection sqref="A1:G369"/>
+      <selection activeCell="J84" sqref="J84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2560,7 +2555,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="2" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2583,7 +2578,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2606,7 +2601,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2629,7 +2624,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2666,7 +2661,7 @@
       <c r="P5" s="21"/>
       <c r="Q5" s="21"/>
     </row>
-    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -2706,7 +2701,7 @@
       <c r="P6" s="21"/>
       <c r="Q6" s="21"/>
     </row>
-    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -2738,7 +2733,7 @@
       <c r="P7" s="21"/>
       <c r="Q7" s="21"/>
     </row>
-    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -2770,7 +2765,7 @@
       <c r="P8" s="21"/>
       <c r="Q8" s="21"/>
     </row>
-    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
@@ -2802,7 +2797,7 @@
       <c r="P9" s="21"/>
       <c r="Q9" s="21"/>
     </row>
-    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
@@ -2841,7 +2836,7 @@
       <c r="P10" s="21"/>
       <c r="Q10" s="21"/>
     </row>
-    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
@@ -2881,7 +2876,7 @@
       <c r="P11" s="21"/>
       <c r="Q11" s="21"/>
     </row>
-    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -2921,7 +2916,7 @@
       <c r="P12" s="21"/>
       <c r="Q12" s="21"/>
     </row>
-    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -2953,7 +2948,7 @@
       <c r="P13" s="21"/>
       <c r="Q13" s="21"/>
     </row>
-    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -2985,7 +2980,7 @@
       <c r="P14" s="21"/>
       <c r="Q14" s="21"/>
     </row>
-    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
@@ -3017,7 +3012,7 @@
       <c r="P15" s="21"/>
       <c r="Q15" s="21"/>
     </row>
-    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
@@ -3049,7 +3044,7 @@
       <c r="P16" s="21"/>
       <c r="Q16" s="21"/>
     </row>
-    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
@@ -3081,7 +3076,7 @@
       <c r="P17" s="21"/>
       <c r="Q17" s="21"/>
     </row>
-    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
@@ -3113,7 +3108,7 @@
       <c r="P18" s="21"/>
       <c r="Q18" s="21"/>
     </row>
-    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>0</v>
       </c>
@@ -3145,7 +3140,7 @@
       <c r="P19" s="21"/>
       <c r="Q19" s="21"/>
     </row>
-    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>0</v>
       </c>
@@ -3177,7 +3172,7 @@
       <c r="P20" s="21"/>
       <c r="Q20" s="21"/>
     </row>
-    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
@@ -3209,7 +3204,7 @@
       <c r="P21" s="21"/>
       <c r="Q21" s="21"/>
     </row>
-    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>0</v>
       </c>
@@ -3273,7 +3268,7 @@
       <c r="P23" s="21"/>
       <c r="Q23" s="21"/>
     </row>
-    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>0</v>
       </c>
@@ -3305,7 +3300,7 @@
       <c r="P24" s="21"/>
       <c r="Q24" s="21"/>
     </row>
-    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>0</v>
       </c>
@@ -3337,7 +3332,7 @@
       <c r="P25" s="21"/>
       <c r="Q25" s="21"/>
     </row>
-    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>0</v>
       </c>
@@ -3369,7 +3364,7 @@
       <c r="P26" s="21"/>
       <c r="Q26" s="21"/>
     </row>
-    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>0</v>
       </c>
@@ -3401,7 +3396,7 @@
       <c r="P27" s="21"/>
       <c r="Q27" s="21"/>
     </row>
-    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>0</v>
       </c>
@@ -3424,7 +3419,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>0</v>
       </c>
@@ -3447,7 +3442,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>0</v>
       </c>
@@ -3516,7 +3511,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>0</v>
       </c>
@@ -3539,7 +3534,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
@@ -3562,7 +3557,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>0</v>
       </c>
@@ -3585,7 +3580,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>0</v>
       </c>
@@ -3608,7 +3603,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>0</v>
       </c>
@@ -3631,7 +3626,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>0</v>
       </c>
@@ -3654,7 +3649,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>0</v>
       </c>
@@ -3677,7 +3672,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>0</v>
       </c>
@@ -3700,7 +3695,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>0</v>
       </c>
@@ -3723,7 +3718,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>0</v>
       </c>
@@ -3746,7 +3741,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>0</v>
       </c>
@@ -3769,7 +3764,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>0</v>
       </c>
@@ -3792,7 +3787,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>0</v>
       </c>
@@ -3815,7 +3810,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>0</v>
       </c>
@@ -3838,7 +3833,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>0</v>
       </c>
@@ -3861,7 +3856,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>0</v>
       </c>
@@ -3884,7 +3879,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>0</v>
       </c>
@@ -3907,7 +3902,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>0</v>
       </c>
@@ -3930,7 +3925,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>0</v>
       </c>
@@ -3953,7 +3948,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>0</v>
       </c>
@@ -3999,7 +3994,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>0</v>
       </c>
@@ -4045,7 +4040,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>0</v>
       </c>
@@ -4068,7 +4063,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>0</v>
       </c>
@@ -4091,7 +4086,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>0</v>
       </c>
@@ -4114,7 +4109,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>0</v>
       </c>
@@ -4137,7 +4132,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>0</v>
       </c>
@@ -4160,7 +4155,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>0</v>
       </c>
@@ -4183,7 +4178,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>0</v>
       </c>
@@ -4206,7 +4201,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>0</v>
       </c>
@@ -4229,7 +4224,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>0</v>
       </c>
@@ -4252,7 +4247,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>0</v>
       </c>
@@ -4275,7 +4270,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>0</v>
       </c>
@@ -4298,7 +4293,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>0</v>
       </c>
@@ -4321,7 +4316,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>0</v>
       </c>
@@ -4344,7 +4339,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>0</v>
       </c>
@@ -4367,7 +4362,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>0</v>
       </c>
@@ -4390,7 +4385,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>0</v>
       </c>
@@ -4413,7 +4408,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>0</v>
       </c>
@@ -4436,7 +4431,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>77</v>
       </c>
@@ -4459,7 +4454,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>77</v>
       </c>
@@ -4482,7 +4477,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>77</v>
       </c>
@@ -4505,7 +4500,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>77</v>
       </c>
@@ -4528,7 +4523,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -4551,7 +4546,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -4574,7 +4569,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>77</v>
       </c>
@@ -4597,7 +4592,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>77</v>
       </c>
@@ -4620,7 +4615,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>77</v>
       </c>
@@ -4643,7 +4638,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>77</v>
       </c>
@@ -4666,7 +4661,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>77</v>
       </c>
@@ -4712,7 +4707,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>77</v>
       </c>
@@ -4758,7 +4753,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>77</v>
       </c>
@@ -4781,7 +4776,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>77</v>
       </c>
@@ -4804,7 +4799,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>77</v>
       </c>
@@ -4827,7 +4822,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>77</v>
       </c>
@@ -4850,7 +4845,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>77</v>
       </c>
@@ -4873,7 +4868,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>77</v>
       </c>
@@ -4896,7 +4891,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>77</v>
       </c>
@@ -4919,7 +4914,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>77</v>
       </c>
@@ -4942,7 +4937,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>77</v>
       </c>
@@ -4965,7 +4960,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>77</v>
       </c>
@@ -4988,7 +4983,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>77</v>
       </c>
@@ -5011,7 +5006,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>77</v>
       </c>
@@ -5034,7 +5029,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>77</v>
       </c>
@@ -5057,7 +5052,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>77</v>
       </c>
@@ -5080,7 +5075,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>77</v>
       </c>
@@ -5103,7 +5098,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>77</v>
       </c>
@@ -5126,7 +5121,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>77</v>
       </c>
@@ -5149,7 +5144,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>77</v>
       </c>
@@ -5172,7 +5167,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>77</v>
       </c>
@@ -5195,7 +5190,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>77</v>
       </c>
@@ -5218,7 +5213,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>77</v>
       </c>
@@ -5264,7 +5259,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>77</v>
       </c>
@@ -5287,7 +5282,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>77</v>
       </c>
@@ -5310,7 +5305,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>77</v>
       </c>
@@ -5333,7 +5328,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>77</v>
       </c>
@@ -5356,7 +5351,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>77</v>
       </c>
@@ -5379,7 +5374,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>77</v>
       </c>
@@ -5402,7 +5397,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>77</v>
       </c>
@@ -5425,7 +5420,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>77</v>
       </c>
@@ -5448,7 +5443,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>77</v>
       </c>
@@ -5471,7 +5466,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>77</v>
       </c>
@@ -5494,7 +5489,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>77</v>
       </c>
@@ -5517,7 +5512,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>77</v>
       </c>
@@ -5540,7 +5535,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>191</v>
       </c>
@@ -5563,7 +5558,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>191</v>
       </c>
@@ -5586,7 +5581,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>191</v>
       </c>
@@ -5609,7 +5604,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>191</v>
       </c>
@@ -5632,7 +5627,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>191</v>
       </c>
@@ -5655,7 +5650,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>191</v>
       </c>
@@ -5678,7 +5673,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>191</v>
       </c>
@@ -5701,7 +5696,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>191</v>
       </c>
@@ -5724,7 +5719,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>191</v>
       </c>
@@ -5747,7 +5742,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>191</v>
       </c>
@@ -5770,7 +5765,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>191</v>
       </c>
@@ -5793,7 +5788,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>191</v>
       </c>
@@ -5816,7 +5811,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>191</v>
       </c>
@@ -5839,7 +5834,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>191</v>
       </c>
@@ -5862,7 +5857,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>191</v>
       </c>
@@ -5885,7 +5880,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>191</v>
       </c>
@@ -5908,7 +5903,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>191</v>
       </c>
@@ -5931,7 +5926,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>191</v>
       </c>
@@ -5954,7 +5949,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>191</v>
       </c>
@@ -5977,7 +5972,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>191</v>
       </c>
@@ -6000,7 +5995,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>191</v>
       </c>
@@ -6023,7 +6018,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>191</v>
       </c>
@@ -6046,7 +6041,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>191</v>
       </c>
@@ -6069,7 +6064,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>191</v>
       </c>
@@ -6092,7 +6087,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>191</v>
       </c>
@@ -6115,7 +6110,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>191</v>
       </c>
@@ -6138,7 +6133,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>191</v>
       </c>
@@ -6184,7 +6179,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>191</v>
       </c>
@@ -6207,7 +6202,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>191</v>
       </c>
@@ -6253,7 +6248,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>191</v>
       </c>
@@ -6276,7 +6271,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>191</v>
       </c>
@@ -6299,7 +6294,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>191</v>
       </c>
@@ -6322,7 +6317,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>191</v>
       </c>
@@ -6345,7 +6340,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>191</v>
       </c>
@@ -6368,7 +6363,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>191</v>
       </c>
@@ -6391,7 +6386,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="158" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>191</v>
       </c>
@@ -6414,7 +6409,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>191</v>
       </c>
@@ -6437,7 +6432,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="160" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>191</v>
       </c>
@@ -6460,7 +6455,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>191</v>
       </c>
@@ -6483,7 +6478,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="162" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>191</v>
       </c>
@@ -6506,7 +6501,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="163" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>191</v>
       </c>
@@ -6529,7 +6524,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="164" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>191</v>
       </c>
@@ -6552,7 +6547,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="165" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>191</v>
       </c>
@@ -6575,7 +6570,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="166" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>191</v>
       </c>
@@ -6598,7 +6593,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="167" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>191</v>
       </c>
@@ -6621,7 +6616,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="168" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>191</v>
       </c>
@@ -6644,7 +6639,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="169" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>191</v>
       </c>
@@ -6667,7 +6662,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="170" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>191</v>
       </c>
@@ -6690,7 +6685,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="171" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>191</v>
       </c>
@@ -6713,7 +6708,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="172" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>191</v>
       </c>
@@ -6736,7 +6731,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>191</v>
       </c>
@@ -6759,7 +6754,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="174" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>191</v>
       </c>
@@ -6782,7 +6777,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="175" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>191</v>
       </c>
@@ -6805,7 +6800,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>191</v>
       </c>
@@ -6828,7 +6823,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="177" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>191</v>
       </c>
@@ -6851,7 +6846,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="178" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>191</v>
       </c>
@@ -6874,7 +6869,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="179" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>191</v>
       </c>
@@ -6897,7 +6892,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="180" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>191</v>
       </c>
@@ -6920,7 +6915,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="181" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>191</v>
       </c>
@@ -6943,7 +6938,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>191</v>
       </c>
@@ -6966,7 +6961,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="183" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>191</v>
       </c>
@@ -6989,7 +6984,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="184" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>191</v>
       </c>
@@ -7012,7 +7007,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="185" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>191</v>
       </c>
@@ -7035,7 +7030,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="186" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>191</v>
       </c>
@@ -7058,7 +7053,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="187" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>192</v>
       </c>
@@ -7081,7 +7076,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>192</v>
       </c>
@@ -7104,7 +7099,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="189" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>192</v>
       </c>
@@ -7127,7 +7122,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>192</v>
       </c>
@@ -7150,7 +7145,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>192</v>
       </c>
@@ -7173,7 +7168,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="192" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>192</v>
       </c>
@@ -7196,7 +7191,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="193" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>192</v>
       </c>
@@ -7219,7 +7214,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="194" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>192</v>
       </c>
@@ -7242,7 +7237,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="195" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>192</v>
       </c>
@@ -7265,7 +7260,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="196" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>192</v>
       </c>
@@ -7288,7 +7283,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="197" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>192</v>
       </c>
@@ -7311,7 +7306,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="198" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>192</v>
       </c>
@@ -7334,7 +7329,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="199" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>192</v>
       </c>
@@ -7357,7 +7352,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="200" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>192</v>
       </c>
@@ -7380,7 +7375,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="201" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>192</v>
       </c>
@@ -7403,7 +7398,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="202" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>192</v>
       </c>
@@ -7426,7 +7421,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="203" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>192</v>
       </c>
@@ -7449,7 +7444,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="204" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>192</v>
       </c>
@@ -7472,7 +7467,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="205" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>192</v>
       </c>
@@ -7495,7 +7490,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="206" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>192</v>
       </c>
@@ -7518,7 +7513,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="207" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>192</v>
       </c>
@@ -7541,7 +7536,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="208" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>192</v>
       </c>
@@ -7564,7 +7559,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="209" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>192</v>
       </c>
@@ -7587,7 +7582,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="210" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>192</v>
       </c>
@@ -7610,7 +7605,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="211" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>192</v>
       </c>
@@ -7633,7 +7628,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="212" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>192</v>
       </c>
@@ -7656,7 +7651,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="213" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>192</v>
       </c>
@@ -7679,7 +7674,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="214" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>192</v>
       </c>
@@ -7702,7 +7697,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="215" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>192</v>
       </c>
@@ -7725,7 +7720,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="216" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>192</v>
       </c>
@@ -7748,7 +7743,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="217" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>192</v>
       </c>
@@ -7771,7 +7766,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="218" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>192</v>
       </c>
@@ -7794,7 +7789,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="219" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>192</v>
       </c>
@@ -7817,7 +7812,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="220" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>192</v>
       </c>
@@ -7840,7 +7835,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="221" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>192</v>
       </c>
@@ -7863,7 +7858,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="222" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>192</v>
       </c>
@@ -7886,7 +7881,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="223" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>192</v>
       </c>
@@ -7909,7 +7904,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="224" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>192</v>
       </c>
@@ -7932,7 +7927,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="225" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>192</v>
       </c>
@@ -7955,7 +7950,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="226" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>192</v>
       </c>
@@ -7978,7 +7973,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="227" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>192</v>
       </c>
@@ -8001,7 +7996,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="228" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>192</v>
       </c>
@@ -8024,7 +8019,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="229" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>192</v>
       </c>
@@ -8047,7 +8042,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="230" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>192</v>
       </c>
@@ -8070,7 +8065,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="231" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>192</v>
       </c>
@@ -8093,7 +8088,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="232" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>192</v>
       </c>
@@ -8116,7 +8111,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="233" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>192</v>
       </c>
@@ -8139,7 +8134,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="234" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>192</v>
       </c>
@@ -8162,7 +8157,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="235" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>192</v>
       </c>
@@ -8185,7 +8180,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="236" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>192</v>
       </c>
@@ -8208,7 +8203,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="237" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>192</v>
       </c>
@@ -8231,7 +8226,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="238" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>192</v>
       </c>
@@ -8254,7 +8249,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="239" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>192</v>
       </c>
@@ -8277,7 +8272,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="240" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>192</v>
       </c>
@@ -8300,7 +8295,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="241" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>192</v>
       </c>
@@ -8323,7 +8318,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="242" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>192</v>
       </c>
@@ -8369,7 +8364,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="244" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>192</v>
       </c>
@@ -8392,7 +8387,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="245" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>192</v>
       </c>
@@ -8415,7 +8410,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="246" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>192</v>
       </c>
@@ -8461,7 +8456,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="248" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>192</v>
       </c>
@@ -8484,7 +8479,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="249" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>192</v>
       </c>
@@ -8507,7 +8502,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="250" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>192</v>
       </c>
@@ -8530,7 +8525,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="251" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>192</v>
       </c>
@@ -8553,7 +8548,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="252" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>192</v>
       </c>
@@ -8576,7 +8571,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="253" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>192</v>
       </c>
@@ -8599,7 +8594,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="254" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>192</v>
       </c>
@@ -8622,7 +8617,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="255" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>261</v>
       </c>
@@ -8668,7 +8663,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="257" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>261</v>
       </c>
@@ -8691,7 +8686,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="258" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>261</v>
       </c>
@@ -8737,7 +8732,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="260" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>261</v>
       </c>
@@ -8760,7 +8755,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="261" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>261</v>
       </c>
@@ -8783,7 +8778,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="262" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>261</v>
       </c>
@@ -8806,7 +8801,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="263" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>261</v>
       </c>
@@ -8829,7 +8824,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="264" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>261</v>
       </c>
@@ -8898,7 +8893,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="267" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>261</v>
       </c>
@@ -8921,7 +8916,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="268" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>261</v>
       </c>
@@ -8944,7 +8939,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="269" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>261</v>
       </c>
@@ -8967,7 +8962,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="270" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>261</v>
       </c>
@@ -8990,7 +8985,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="271" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>261</v>
       </c>
@@ -9013,7 +9008,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="272" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>261</v>
       </c>
@@ -9036,7 +9031,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="273" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>261</v>
       </c>
@@ -9059,7 +9054,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="274" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>261</v>
       </c>
@@ -9082,7 +9077,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="275" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>261</v>
       </c>
@@ -9105,7 +9100,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="276" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>261</v>
       </c>
@@ -9128,7 +9123,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="277" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>261</v>
       </c>
@@ -9151,7 +9146,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="278" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>261</v>
       </c>
@@ -9174,7 +9169,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="279" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>261</v>
       </c>
@@ -9197,7 +9192,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="280" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>261</v>
       </c>
@@ -9220,7 +9215,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="281" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>261</v>
       </c>
@@ -9243,7 +9238,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="282" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>261</v>
       </c>
@@ -9266,7 +9261,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="283" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>261</v>
       </c>
@@ -9312,7 +9307,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="285" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>261</v>
       </c>
@@ -9335,7 +9330,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="286" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>261</v>
       </c>
@@ -9358,7 +9353,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="287" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>261</v>
       </c>
@@ -9381,7 +9376,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="288" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>261</v>
       </c>
@@ -9404,7 +9399,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="289" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>261</v>
       </c>
@@ -9427,7 +9422,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="290" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>261</v>
       </c>
@@ -9450,7 +9445,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="291" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>261</v>
       </c>
@@ -9473,7 +9468,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="292" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>261</v>
       </c>
@@ -9496,7 +9491,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="293" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>261</v>
       </c>
@@ -9519,7 +9514,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="294" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>261</v>
       </c>
@@ -9542,7 +9537,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="295" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>261</v>
       </c>
@@ -9565,7 +9560,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="296" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>261</v>
       </c>
@@ -9588,7 +9583,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="297" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>261</v>
       </c>
@@ -9611,7 +9606,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="298" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>261</v>
       </c>
@@ -9634,7 +9629,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="299" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>261</v>
       </c>
@@ -9657,7 +9652,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="300" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>261</v>
       </c>
@@ -9680,7 +9675,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="301" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>261</v>
       </c>
@@ -9703,7 +9698,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="302" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>261</v>
       </c>
@@ -9726,7 +9721,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="303" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>261</v>
       </c>
@@ -9749,7 +9744,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="304" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>261</v>
       </c>
@@ -9772,7 +9767,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="305" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>261</v>
       </c>
@@ -9818,7 +9813,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="307" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>261</v>
       </c>
@@ -9841,7 +9836,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="308" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>261</v>
       </c>
@@ -9864,7 +9859,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="309" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>261</v>
       </c>
@@ -9887,7 +9882,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="310" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>261</v>
       </c>
@@ -9910,7 +9905,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="311" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>261</v>
       </c>
@@ -9933,7 +9928,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="312" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>261</v>
       </c>
@@ -9956,7 +9951,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="313" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>343</v>
       </c>
@@ -9979,7 +9974,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="314" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>343</v>
       </c>
@@ -10002,7 +9997,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="315" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>343</v>
       </c>
@@ -10025,7 +10020,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="316" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>343</v>
       </c>
@@ -10071,7 +10066,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="318" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>343</v>
       </c>
@@ -10094,7 +10089,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="319" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>343</v>
       </c>
@@ -10117,7 +10112,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="320" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>343</v>
       </c>
@@ -10140,7 +10135,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="321" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>343</v>
       </c>
@@ -10163,7 +10158,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="322" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>343</v>
       </c>
@@ -10186,7 +10181,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="323" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>343</v>
       </c>
@@ -10209,7 +10204,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="324" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>343</v>
       </c>
@@ -10232,7 +10227,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="325" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>343</v>
       </c>
@@ -10255,7 +10250,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="326" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>343</v>
       </c>
@@ -10278,7 +10273,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="327" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>343</v>
       </c>
@@ -10301,7 +10296,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="328" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>343</v>
       </c>
@@ -10324,7 +10319,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="329" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>343</v>
       </c>
@@ -10347,7 +10342,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="330" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>343</v>
       </c>
@@ -10370,7 +10365,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="331" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>343</v>
       </c>
@@ -10416,7 +10411,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="333" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>343</v>
       </c>
@@ -10439,7 +10434,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="334" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>343</v>
       </c>
@@ -10462,7 +10457,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="335" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>343</v>
       </c>
@@ -10485,7 +10480,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="336" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>343</v>
       </c>
@@ -10508,7 +10503,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="337" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>343</v>
       </c>
@@ -10531,7 +10526,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="338" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>343</v>
       </c>
@@ -10554,7 +10549,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="339" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>343</v>
       </c>
@@ -10577,7 +10572,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="340" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>343</v>
       </c>
@@ -10600,7 +10595,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="341" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>343</v>
       </c>
@@ -10623,7 +10618,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="342" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>344</v>
       </c>
@@ -10646,7 +10641,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="343" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>344</v>
       </c>
@@ -10669,7 +10664,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="344" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>344</v>
       </c>
@@ -10692,7 +10687,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="345" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>344</v>
       </c>
@@ -10715,7 +10710,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="346" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>344</v>
       </c>
@@ -10738,7 +10733,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="347" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>344</v>
       </c>
@@ -10761,7 +10756,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="348" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>344</v>
       </c>
@@ -10784,7 +10779,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="349" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>344</v>
       </c>
@@ -10807,7 +10802,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="350" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>344</v>
       </c>
@@ -10830,7 +10825,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="351" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>344</v>
       </c>
@@ -10853,7 +10848,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="352" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>344</v>
       </c>
@@ -10876,7 +10871,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="353" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>344</v>
       </c>
@@ -10899,7 +10894,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="354" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>344</v>
       </c>
@@ -10922,7 +10917,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="355" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>344</v>
       </c>
@@ -10945,7 +10940,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="356" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>344</v>
       </c>
@@ -10968,7 +10963,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="357" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>344</v>
       </c>
@@ -10991,7 +10986,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="358" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>344</v>
       </c>
@@ -11014,7 +11009,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="359" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>344</v>
       </c>
@@ -11060,7 +11055,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="361" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>344</v>
       </c>
@@ -11083,7 +11078,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="362" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>344</v>
       </c>
@@ -11106,7 +11101,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="363" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>344</v>
       </c>
@@ -11129,7 +11124,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="364" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>344</v>
       </c>
@@ -11152,7 +11147,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="365" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>344</v>
       </c>
@@ -11175,7 +11170,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="366" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>344</v>
       </c>
@@ -11221,7 +11216,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="368" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>344</v>
       </c>
@@ -11267,7 +11262,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="370" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>344</v>
       </c>
@@ -11290,7 +11285,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="371" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>344</v>
       </c>
@@ -11313,7 +11308,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="372" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>344</v>
       </c>
@@ -11336,7 +11331,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="373" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>344</v>
       </c>

</xml_diff>